<commit_message>
Java3D Update, rules for galactolipids, bugfixes oxlipids
</commit_message>
<xml_diff>
--- a/fattyAcids/fattyAcidChains.xlsx
+++ b/fattyAcids/fattyAcidChains.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="4695" yWindow="60" windowWidth="15195" windowHeight="12525"/>
+    <workbookView xWindow="-120" yWindow="288" windowWidth="23256" windowHeight="13176"/>
   </bookViews>
   <sheets>
     <sheet name="FAS" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="9">
   <si>
     <t>:</t>
   </si>
@@ -35,6 +35,12 @@
   </si>
   <si>
     <t>O</t>
+  </si>
+  <si>
+    <t>;O1;O2;O3;O4;X1;X2,X3,X4;X1,O1;O2,X1;X2,O1</t>
+  </si>
+  <si>
+    <t>PSM</t>
   </si>
 </sst>
 </file>
@@ -118,7 +124,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -126,14 +132,17 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Larissa">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -171,7 +180,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Larissa">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -243,7 +252,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Larissa">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -419,19 +428,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:L163"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="7" width="11.42578125" customWidth="1"/>
-    <col min="8" max="8" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="11" width="11.42578125" customWidth="1"/>
-    <col min="12" max="12" width="16.140625" customWidth="1"/>
+    <col min="1" max="7" width="11.44140625" customWidth="1"/>
+    <col min="8" max="8" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="11.44140625" customWidth="1"/>
+    <col min="12" max="12" width="16.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -451,8 +460,11 @@
       <c r="G2" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H2" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -474,8 +486,11 @@
       <c r="G3" s="5">
         <v>60.021120547999999</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -497,8 +512,11 @@
       <c r="G4" s="5">
         <v>74.036770582000003</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -520,8 +538,11 @@
       <c r="G5" s="5">
         <v>88.052420616000006</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -543,8 +564,11 @@
       <c r="G6" s="5">
         <v>102.06807070000001</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -566,8 +590,11 @@
       <c r="G7" s="5">
         <v>116.08372068399999</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -589,8 +616,11 @@
       <c r="G8" s="5">
         <v>130.09937071799999</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -612,8 +642,11 @@
       <c r="G9" s="5">
         <v>144.11502075199999</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -635,8 +668,11 @@
       <c r="G10" s="5">
         <v>158.130670786</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -658,8 +694,11 @@
       <c r="G11" s="5">
         <v>172.14632082</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -681,8 +720,11 @@
       <c r="G12" s="5">
         <v>186.161970854</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -704,8 +746,11 @@
       <c r="G13" s="5">
         <v>200.17762088799998</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H13" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -727,8 +772,11 @@
       <c r="G14" s="5">
         <v>214.19327092199998</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -750,8 +798,11 @@
       <c r="G15" s="5">
         <v>228.20892095599999</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H15" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -773,8 +824,11 @@
       <c r="G16" s="5">
         <v>242.22457098999999</v>
       </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="H16" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -796,10 +850,13 @@
       <c r="G17" s="5">
         <v>256.24022102399999</v>
       </c>
+      <c r="H17" t="s">
+        <v>7</v>
+      </c>
       <c r="K17" s="6"/>
       <c r="L17" s="7"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -821,10 +878,13 @@
       <c r="G18" s="5">
         <v>270.25587105800003</v>
       </c>
+      <c r="H18" t="s">
+        <v>7</v>
+      </c>
       <c r="K18" s="6"/>
       <c r="L18" s="7"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -846,10 +906,13 @@
       <c r="G19" s="5">
         <v>284.271521092</v>
       </c>
+      <c r="H19" t="s">
+        <v>7</v>
+      </c>
       <c r="K19" s="6"/>
       <c r="L19" s="7"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -871,10 +934,13 @@
       <c r="G20" s="5">
         <v>298.28717112599998</v>
       </c>
+      <c r="H20" t="s">
+        <v>7</v>
+      </c>
       <c r="K20" s="6"/>
       <c r="L20" s="7"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>20</v>
       </c>
@@ -896,10 +962,13 @@
       <c r="G21" s="5">
         <v>312.30282116000001</v>
       </c>
+      <c r="H21" t="s">
+        <v>7</v>
+      </c>
       <c r="K21" s="6"/>
       <c r="L21" s="7"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>21</v>
       </c>
@@ -921,10 +990,13 @@
       <c r="G22" s="5">
         <v>326.31847119399998</v>
       </c>
+      <c r="H22" t="s">
+        <v>7</v>
+      </c>
       <c r="K22" s="6"/>
       <c r="L22" s="7"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>22</v>
       </c>
@@ -946,10 +1018,13 @@
       <c r="G23" s="5">
         <v>340.33412122800001</v>
       </c>
+      <c r="H23" t="s">
+        <v>7</v>
+      </c>
       <c r="K23" s="6"/>
       <c r="L23" s="8"/>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>23</v>
       </c>
@@ -971,10 +1046,13 @@
       <c r="G24" s="5">
         <v>354.34977126199999</v>
       </c>
+      <c r="H24" t="s">
+        <v>7</v>
+      </c>
       <c r="K24" s="6"/>
       <c r="L24" s="8"/>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>24</v>
       </c>
@@ -996,8 +1074,11 @@
       <c r="G25" s="5">
         <v>368.36542129599997</v>
       </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="H25" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>25</v>
       </c>
@@ -1019,8 +1100,11 @@
       <c r="G26" s="5">
         <v>382.38107133</v>
       </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="H26" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>26</v>
       </c>
@@ -1042,8 +1126,11 @@
       <c r="G27" s="5">
         <v>396.39672136399997</v>
       </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="H27" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>27</v>
       </c>
@@ -1065,8 +1152,11 @@
       <c r="G28" s="5">
         <v>410.412371398</v>
       </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="H28" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>28</v>
       </c>
@@ -1088,8 +1178,11 @@
       <c r="G29" s="5">
         <v>424.42802143199998</v>
       </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="H29" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>29</v>
       </c>
@@ -1111,8 +1204,11 @@
       <c r="G30" s="5">
         <v>438.44367146600001</v>
       </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="H30" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>30</v>
       </c>
@@ -1134,8 +1230,11 @@
       <c r="G31" s="5">
         <v>452.45932149999999</v>
       </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="H31" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="9"/>
       <c r="B32" s="10"/>
       <c r="C32" s="11"/>
@@ -1144,7 +1243,7 @@
       <c r="F32" s="10"/>
       <c r="G32" s="12"/>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>10</v>
       </c>
@@ -1166,8 +1265,11 @@
       <c r="G33" s="5">
         <v>170.130670786</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H33" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>11</v>
       </c>
@@ -1189,8 +1291,11 @@
       <c r="G34" s="5">
         <v>184.14632082</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H34" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>12</v>
       </c>
@@ -1212,8 +1317,11 @@
       <c r="G35" s="5">
         <v>198.161970854</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H35" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>13</v>
       </c>
@@ -1235,8 +1343,11 @@
       <c r="G36" s="5">
         <v>212.17762088799998</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H36" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>14</v>
       </c>
@@ -1258,8 +1369,11 @@
       <c r="G37" s="5">
         <v>226.19327092199998</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H37" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>15</v>
       </c>
@@ -1281,8 +1395,11 @@
       <c r="G38" s="5">
         <v>240.20892095599999</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H38" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>16</v>
       </c>
@@ -1304,8 +1421,11 @@
       <c r="G39" s="5">
         <v>254.22457098999999</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H39" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>17</v>
       </c>
@@ -1327,8 +1447,11 @@
       <c r="G40" s="5">
         <v>268.24022102399999</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H40" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>18</v>
       </c>
@@ -1350,8 +1473,11 @@
       <c r="G41" s="5">
         <v>282.25587105800003</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H41" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>19</v>
       </c>
@@ -1373,8 +1499,11 @@
       <c r="G42" s="5">
         <v>296.271521092</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H42" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>20</v>
       </c>
@@ -1396,8 +1525,11 @@
       <c r="G43" s="5">
         <v>310.28717112599998</v>
       </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H43" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>21</v>
       </c>
@@ -1419,8 +1551,11 @@
       <c r="G44" s="5">
         <v>324.30282116000001</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H44" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>22</v>
       </c>
@@ -1442,8 +1577,11 @@
       <c r="G45" s="5">
         <v>338.31847119399998</v>
       </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H45" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>23</v>
       </c>
@@ -1465,8 +1603,11 @@
       <c r="G46" s="5">
         <v>352.33412122800001</v>
       </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H46" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <v>24</v>
       </c>
@@ -1488,8 +1629,11 @@
       <c r="G47" s="5">
         <v>366.34977126199999</v>
       </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H47" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
         <v>25</v>
       </c>
@@ -1511,8 +1655,11 @@
       <c r="G48" s="5">
         <v>380.36542129599997</v>
       </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H48" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <v>26</v>
       </c>
@@ -1534,8 +1681,11 @@
       <c r="G49" s="5">
         <v>394.38107133</v>
       </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H49" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
         <v>27</v>
       </c>
@@ -1557,8 +1707,11 @@
       <c r="G50" s="5">
         <v>408.39672136399997</v>
       </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H50" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
         <v>28</v>
       </c>
@@ -1580,8 +1733,11 @@
       <c r="G51" s="5">
         <v>422.412371398</v>
       </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H51" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
         <v>29</v>
       </c>
@@ -1603,8 +1759,11 @@
       <c r="G52" s="5">
         <v>436.42802143199998</v>
       </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H52" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
         <v>30</v>
       </c>
@@ -1626,8 +1785,11 @@
       <c r="G53" s="5">
         <v>450.44367146600001</v>
       </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H53" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="6"/>
       <c r="B54" s="6"/>
       <c r="C54" s="6"/>
@@ -1636,7 +1798,7 @@
       <c r="F54" s="6"/>
       <c r="G54" s="6"/>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
         <v>10</v>
       </c>
@@ -1658,8 +1820,11 @@
       <c r="G55" s="5">
         <v>168.11502075199999</v>
       </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H55" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
         <v>11</v>
       </c>
@@ -1681,8 +1846,11 @@
       <c r="G56" s="5">
         <v>182.130670786</v>
       </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H56" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
         <v>12</v>
       </c>
@@ -1704,8 +1872,11 @@
       <c r="G57" s="5">
         <v>196.14632082</v>
       </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H57" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
         <v>13</v>
       </c>
@@ -1727,8 +1898,11 @@
       <c r="G58" s="5">
         <v>210.161970854</v>
       </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H58" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
         <v>14</v>
       </c>
@@ -1750,8 +1924,11 @@
       <c r="G59" s="5">
         <v>224.17762088799998</v>
       </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H59" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
         <v>15</v>
       </c>
@@ -1773,8 +1950,11 @@
       <c r="G60" s="5">
         <v>238.19327092199998</v>
       </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H60" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="2">
         <v>16</v>
       </c>
@@ -1796,8 +1976,11 @@
       <c r="G61" s="5">
         <v>252.20892095599999</v>
       </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H61" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
         <v>17</v>
       </c>
@@ -1819,8 +2002,11 @@
       <c r="G62" s="5">
         <v>266.22457099000002</v>
       </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H62" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="2">
         <v>18</v>
       </c>
@@ -1842,8 +2028,11 @@
       <c r="G63" s="5">
         <v>280.24022102399999</v>
       </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H63" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="2">
         <v>19</v>
       </c>
@@ -1865,8 +2054,11 @@
       <c r="G64" s="5">
         <v>294.25587105799997</v>
       </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H64" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
         <v>20</v>
       </c>
@@ -1888,8 +2080,11 @@
       <c r="G65" s="5">
         <v>308.271521092</v>
       </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H65" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="2">
         <v>21</v>
       </c>
@@ -1911,8 +2106,11 @@
       <c r="G66" s="5">
         <v>322.28717112599998</v>
       </c>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H66" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="2">
         <v>22</v>
       </c>
@@ -1934,8 +2132,11 @@
       <c r="G67" s="5">
         <v>336.30282116000001</v>
       </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H67" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="2">
         <v>23</v>
       </c>
@@ -1957,8 +2158,11 @@
       <c r="G68" s="5">
         <v>350.31847119399998</v>
       </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H68" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="2">
         <v>24</v>
       </c>
@@ -1980,8 +2184,11 @@
       <c r="G69" s="5">
         <v>364.33412122800001</v>
       </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H69" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="2">
         <v>25</v>
       </c>
@@ -2003,8 +2210,11 @@
       <c r="G70" s="5">
         <v>378.34977126199999</v>
       </c>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H70" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="2">
         <v>26</v>
       </c>
@@ -2026,8 +2236,11 @@
       <c r="G71" s="5">
         <v>392.36542129599997</v>
       </c>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H71" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="2">
         <v>27</v>
       </c>
@@ -2049,8 +2262,11 @@
       <c r="G72" s="5">
         <v>406.38107133</v>
       </c>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H72" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="2">
         <v>28</v>
       </c>
@@ -2072,8 +2288,11 @@
       <c r="G73" s="5">
         <v>420.39672136399997</v>
       </c>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H73" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="2">
         <v>29</v>
       </c>
@@ -2095,8 +2314,11 @@
       <c r="G74" s="5">
         <v>434.412371398</v>
       </c>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H74" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="2">
         <v>30</v>
       </c>
@@ -2118,8 +2340,11 @@
       <c r="G75" s="5">
         <v>448.42802143199998</v>
       </c>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H75" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="6"/>
       <c r="B76" s="6"/>
       <c r="C76" s="6"/>
@@ -2128,7 +2353,7 @@
       <c r="F76" s="6"/>
       <c r="G76" s="6"/>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="2">
         <v>10</v>
       </c>
@@ -2150,8 +2375,11 @@
       <c r="G77" s="5">
         <v>166.09937071799999</v>
       </c>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H77" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="2">
         <v>11</v>
       </c>
@@ -2173,8 +2401,11 @@
       <c r="G78" s="5">
         <v>180.11502075199999</v>
       </c>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H78" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="2">
         <v>12</v>
       </c>
@@ -2196,8 +2427,11 @@
       <c r="G79" s="5">
         <v>194.130670786</v>
       </c>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H79" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="2">
         <v>13</v>
       </c>
@@ -2219,8 +2453,11 @@
       <c r="G80" s="5">
         <v>208.14632082</v>
       </c>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H80" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="2">
         <v>14</v>
       </c>
@@ -2242,8 +2479,11 @@
       <c r="G81" s="5">
         <v>222.161970854</v>
       </c>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H81" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="2">
         <v>15</v>
       </c>
@@ -2265,8 +2505,11 @@
       <c r="G82" s="5">
         <v>236.17762088799998</v>
       </c>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H82" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="2">
         <v>16</v>
       </c>
@@ -2288,8 +2531,11 @@
       <c r="G83" s="5">
         <v>250.19327092199998</v>
       </c>
-    </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H83" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="2">
         <v>17</v>
       </c>
@@ -2311,8 +2557,11 @@
       <c r="G84" s="5">
         <v>264.20892095599999</v>
       </c>
-    </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H84" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="2">
         <v>18</v>
       </c>
@@ -2334,8 +2583,11 @@
       <c r="G85" s="5">
         <v>278.22457099000002</v>
       </c>
-    </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H85" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="2">
         <v>19</v>
       </c>
@@ -2357,8 +2609,11 @@
       <c r="G86" s="5">
         <v>292.24022102399999</v>
       </c>
-    </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H86" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" s="2">
         <v>20</v>
       </c>
@@ -2380,8 +2635,11 @@
       <c r="G87" s="5">
         <v>306.25587105799997</v>
       </c>
-    </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H87" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" s="2">
         <v>21</v>
       </c>
@@ -2403,8 +2661,11 @@
       <c r="G88" s="5">
         <v>320.271521092</v>
       </c>
-    </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H88" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" s="2">
         <v>22</v>
       </c>
@@ -2426,8 +2687,11 @@
       <c r="G89" s="5">
         <v>334.28717112599998</v>
       </c>
-    </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H89" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" s="2">
         <v>23</v>
       </c>
@@ -2449,8 +2713,11 @@
       <c r="G90" s="5">
         <v>348.30282116000001</v>
       </c>
-    </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H90" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" s="2">
         <v>24</v>
       </c>
@@ -2472,8 +2739,11 @@
       <c r="G91" s="5">
         <v>362.31847119399998</v>
       </c>
-    </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H91" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" s="2">
         <v>25</v>
       </c>
@@ -2495,8 +2765,11 @@
       <c r="G92" s="5">
         <v>376.33412122800001</v>
       </c>
-    </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H92" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" s="2">
         <v>26</v>
       </c>
@@ -2518,8 +2791,11 @@
       <c r="G93" s="5">
         <v>390.34977126199999</v>
       </c>
-    </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H93" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" s="2">
         <v>27</v>
       </c>
@@ -2541,8 +2817,11 @@
       <c r="G94" s="5">
         <v>404.36542129599997</v>
       </c>
-    </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H94" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" s="2">
         <v>28</v>
       </c>
@@ -2564,8 +2843,11 @@
       <c r="G95" s="5">
         <v>418.38107133</v>
       </c>
-    </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H95" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" s="2">
         <v>29</v>
       </c>
@@ -2587,8 +2869,11 @@
       <c r="G96" s="5">
         <v>432.39672136399997</v>
       </c>
-    </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H96" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" s="2">
         <v>30</v>
       </c>
@@ -2610,8 +2895,11 @@
       <c r="G97" s="5">
         <v>446.412371398</v>
       </c>
-    </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H97" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" s="6"/>
       <c r="B98" s="6"/>
       <c r="C98" s="6"/>
@@ -2620,7 +2908,7 @@
       <c r="F98" s="6"/>
       <c r="G98" s="6"/>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" s="2">
         <v>10</v>
       </c>
@@ -2642,8 +2930,11 @@
       <c r="G99" s="5">
         <v>164.08372068399999</v>
       </c>
-    </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H99" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" s="2">
         <v>11</v>
       </c>
@@ -2665,8 +2956,11 @@
       <c r="G100" s="5">
         <v>178.09937071799999</v>
       </c>
-    </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H100" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101" s="2">
         <v>12</v>
       </c>
@@ -2688,8 +2982,11 @@
       <c r="G101" s="5">
         <v>192.11502075199999</v>
       </c>
-    </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H101" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102" s="2">
         <v>13</v>
       </c>
@@ -2711,8 +3008,11 @@
       <c r="G102" s="5">
         <v>206.130670786</v>
       </c>
-    </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H102" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103" s="2">
         <v>14</v>
       </c>
@@ -2734,8 +3034,11 @@
       <c r="G103" s="5">
         <v>220.14632082</v>
       </c>
-    </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H103" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A104" s="2">
         <v>15</v>
       </c>
@@ -2757,8 +3060,11 @@
       <c r="G104" s="5">
         <v>234.161970854</v>
       </c>
-    </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H104" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105" s="2">
         <v>16</v>
       </c>
@@ -2780,8 +3086,11 @@
       <c r="G105" s="5">
         <v>248.17762088799998</v>
       </c>
-    </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H105" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A106" s="2">
         <v>17</v>
       </c>
@@ -2803,8 +3112,11 @@
       <c r="G106" s="5">
         <v>262.19327092200001</v>
       </c>
-    </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H106" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A107" s="2">
         <v>18</v>
       </c>
@@ -2826,8 +3138,11 @@
       <c r="G107" s="5">
         <v>276.20892095599999</v>
       </c>
-    </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H107" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A108" s="2">
         <v>19</v>
       </c>
@@ -2849,8 +3164,11 @@
       <c r="G108" s="5">
         <v>290.22457099000002</v>
       </c>
-    </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H108" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A109" s="2">
         <v>20</v>
       </c>
@@ -2872,8 +3190,11 @@
       <c r="G109" s="5">
         <v>304.24022102399999</v>
       </c>
-    </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H109" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A110" s="2">
         <v>21</v>
       </c>
@@ -2895,8 +3216,11 @@
       <c r="G110" s="5">
         <v>318.25587105799997</v>
       </c>
-    </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H110" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A111" s="2">
         <v>22</v>
       </c>
@@ -2918,8 +3242,11 @@
       <c r="G111" s="5">
         <v>332.271521092</v>
       </c>
-    </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H111" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A112" s="2">
         <v>23</v>
       </c>
@@ -2941,8 +3268,11 @@
       <c r="G112" s="5">
         <v>346.28717112599998</v>
       </c>
-    </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H112" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A113" s="2">
         <v>24</v>
       </c>
@@ -2964,8 +3294,11 @@
       <c r="G113" s="5">
         <v>360.30282116000001</v>
       </c>
-    </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H113" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A114" s="2">
         <v>25</v>
       </c>
@@ -2987,8 +3320,11 @@
       <c r="G114" s="5">
         <v>374.31847119399998</v>
       </c>
-    </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H114" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A115" s="2">
         <v>26</v>
       </c>
@@ -3010,8 +3346,11 @@
       <c r="G115" s="5">
         <v>388.33412122800001</v>
       </c>
-    </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H115" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A116" s="2">
         <v>27</v>
       </c>
@@ -3033,8 +3372,11 @@
       <c r="G116" s="5">
         <v>402.34977126199999</v>
       </c>
-    </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H116" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A117" s="2">
         <v>28</v>
       </c>
@@ -3056,8 +3398,11 @@
       <c r="G117" s="5">
         <v>416.36542129599997</v>
       </c>
-    </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H117" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A118" s="2">
         <v>29</v>
       </c>
@@ -3079,8 +3424,11 @@
       <c r="G118" s="5">
         <v>430.38107133</v>
       </c>
-    </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H118" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A119" s="2">
         <v>30</v>
       </c>
@@ -3102,8 +3450,11 @@
       <c r="G119" s="5">
         <v>444.39672136399997</v>
       </c>
-    </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H119" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A120" s="6"/>
       <c r="B120" s="6"/>
       <c r="C120" s="6"/>
@@ -3112,7 +3463,7 @@
       <c r="F120" s="6"/>
       <c r="G120" s="6"/>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A121" s="2">
         <v>10</v>
       </c>
@@ -3134,8 +3485,11 @@
       <c r="G121" s="5">
         <v>162.06807064999998</v>
       </c>
-    </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H121" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A122" s="2">
         <v>11</v>
       </c>
@@ -3157,8 +3511,11 @@
       <c r="G122" s="5">
         <v>176.08372068399999</v>
       </c>
-    </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H122" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A123" s="2">
         <v>12</v>
       </c>
@@ -3180,8 +3537,11 @@
       <c r="G123" s="5">
         <v>190.09937071799999</v>
       </c>
-    </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H123" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A124" s="2">
         <v>13</v>
       </c>
@@ -3203,8 +3563,11 @@
       <c r="G124" s="5">
         <v>204.11502075199999</v>
       </c>
-    </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H124" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A125" s="2">
         <v>14</v>
       </c>
@@ -3226,8 +3589,11 @@
       <c r="G125" s="5">
         <v>218.130670786</v>
       </c>
-    </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H125" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A126" s="2">
         <v>15</v>
       </c>
@@ -3249,8 +3615,11 @@
       <c r="G126" s="5">
         <v>232.14632082</v>
       </c>
-    </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H126" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A127" s="2">
         <v>16</v>
       </c>
@@ -3272,8 +3641,11 @@
       <c r="G127" s="5">
         <v>246.161970854</v>
       </c>
-    </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H127" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A128" s="2">
         <v>17</v>
       </c>
@@ -3295,8 +3667,11 @@
       <c r="G128" s="5">
         <v>260.17762088799998</v>
       </c>
-    </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H128" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A129" s="2">
         <v>18</v>
       </c>
@@ -3318,8 +3693,11 @@
       <c r="G129" s="5">
         <v>274.19327092200001</v>
       </c>
-    </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H129" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A130" s="2">
         <v>19</v>
       </c>
@@ -3341,8 +3719,11 @@
       <c r="G130" s="5">
         <v>288.20892095599999</v>
       </c>
-    </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H130" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A131" s="2">
         <v>20</v>
       </c>
@@ -3364,8 +3745,11 @@
       <c r="G131" s="5">
         <v>302.22457099000002</v>
       </c>
-    </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H131" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A132" s="2">
         <v>21</v>
       </c>
@@ -3387,8 +3771,11 @@
       <c r="G132" s="5">
         <v>316.24022102399999</v>
       </c>
-    </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H132" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A133" s="2">
         <v>22</v>
       </c>
@@ -3410,8 +3797,11 @@
       <c r="G133" s="5">
         <v>330.25587105799997</v>
       </c>
-    </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H133" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A134" s="2">
         <v>23</v>
       </c>
@@ -3433,8 +3823,11 @@
       <c r="G134" s="5">
         <v>344.271521092</v>
       </c>
-    </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H134" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A135" s="2">
         <v>24</v>
       </c>
@@ -3456,8 +3849,11 @@
       <c r="G135" s="5">
         <v>358.28717112599998</v>
       </c>
-    </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H135" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A136" s="2">
         <v>25</v>
       </c>
@@ -3479,8 +3875,11 @@
       <c r="G136" s="5">
         <v>372.30282116000001</v>
       </c>
-    </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H136" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A137" s="2">
         <v>26</v>
       </c>
@@ -3502,8 +3901,11 @@
       <c r="G137" s="5">
         <v>386.31847119399998</v>
       </c>
-    </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H137" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A138" s="2">
         <v>27</v>
       </c>
@@ -3525,8 +3927,11 @@
       <c r="G138" s="5">
         <v>400.33412122800001</v>
       </c>
-    </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H138" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A139" s="2">
         <v>28</v>
       </c>
@@ -3548,8 +3953,11 @@
       <c r="G139" s="5">
         <v>414.34977126199999</v>
       </c>
-    </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H139" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A140" s="2">
         <v>29</v>
       </c>
@@ -3571,8 +3979,11 @@
       <c r="G140" s="5">
         <v>428.36542129599997</v>
       </c>
-    </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H140" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A141" s="2">
         <v>30</v>
       </c>
@@ -3594,8 +4005,11 @@
       <c r="G141" s="5">
         <v>442.38107133</v>
       </c>
-    </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H141" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A142" s="6"/>
       <c r="B142" s="6"/>
       <c r="C142" s="6"/>
@@ -3604,7 +4018,7 @@
       <c r="F142" s="6"/>
       <c r="G142" s="6"/>
     </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A143" s="2">
         <v>10</v>
       </c>
@@ -3626,8 +4040,11 @@
       <c r="G143" s="5">
         <v>160.05242061600001</v>
       </c>
-    </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H143" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A144" s="2">
         <v>11</v>
       </c>
@@ -3649,8 +4066,11 @@
       <c r="G144" s="5">
         <v>174.06807064999998</v>
       </c>
-    </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H144" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A145" s="2">
         <v>12</v>
       </c>
@@ -3672,8 +4092,11 @@
       <c r="G145" s="5">
         <v>188.08372068399999</v>
       </c>
-    </row>
-    <row r="146" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H145" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A146" s="2">
         <v>13</v>
       </c>
@@ -3695,8 +4118,11 @@
       <c r="G146" s="5">
         <v>202.09937071799999</v>
       </c>
-    </row>
-    <row r="147" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H146" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A147" s="2">
         <v>14</v>
       </c>
@@ -3718,8 +4144,11 @@
       <c r="G147" s="5">
         <v>216.11502075199999</v>
       </c>
-    </row>
-    <row r="148" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H147" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A148" s="2">
         <v>15</v>
       </c>
@@ -3741,8 +4170,11 @@
       <c r="G148" s="5">
         <v>230.130670786</v>
       </c>
-    </row>
-    <row r="149" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H148" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A149" s="2">
         <v>16</v>
       </c>
@@ -3764,8 +4196,11 @@
       <c r="G149" s="5">
         <v>244.14632082</v>
       </c>
-    </row>
-    <row r="150" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H149" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="150" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A150" s="2">
         <v>17</v>
       </c>
@@ -3787,8 +4222,11 @@
       <c r="G150" s="5">
         <v>258.161970854</v>
       </c>
-    </row>
-    <row r="151" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H150" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A151" s="2">
         <v>18</v>
       </c>
@@ -3810,8 +4248,11 @@
       <c r="G151" s="5">
         <v>272.17762088799998</v>
       </c>
-    </row>
-    <row r="152" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H151" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A152" s="2">
         <v>19</v>
       </c>
@@ -3833,8 +4274,11 @@
       <c r="G152" s="5">
         <v>286.19327092200001</v>
       </c>
-    </row>
-    <row r="153" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H152" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="153" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A153" s="2">
         <v>20</v>
       </c>
@@ -3856,8 +4300,11 @@
       <c r="G153" s="5">
         <v>300.20892095599999</v>
       </c>
-    </row>
-    <row r="154" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H153" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="154" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A154" s="2">
         <v>21</v>
       </c>
@@ -3879,8 +4326,11 @@
       <c r="G154" s="5">
         <v>314.22457099000002</v>
       </c>
-    </row>
-    <row r="155" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H154" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="155" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A155" s="2">
         <v>22</v>
       </c>
@@ -3902,8 +4352,11 @@
       <c r="G155" s="5">
         <v>328.24022102399999</v>
       </c>
-    </row>
-    <row r="156" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H155" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="156" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A156" s="2">
         <v>23</v>
       </c>
@@ -3925,8 +4378,11 @@
       <c r="G156" s="5">
         <v>342.25587105799997</v>
       </c>
-    </row>
-    <row r="157" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H156" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="157" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A157" s="2">
         <v>24</v>
       </c>
@@ -3948,8 +4404,11 @@
       <c r="G157" s="5">
         <v>356.271521092</v>
       </c>
-    </row>
-    <row r="158" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H157" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="158" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A158" s="2">
         <v>25</v>
       </c>
@@ -3971,8 +4430,11 @@
       <c r="G158" s="5">
         <v>370.28717112599998</v>
       </c>
-    </row>
-    <row r="159" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H158" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="159" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A159" s="2">
         <v>26</v>
       </c>
@@ -3994,8 +4456,11 @@
       <c r="G159" s="5">
         <v>384.30282116000001</v>
       </c>
-    </row>
-    <row r="160" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H159" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="160" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A160" s="2">
         <v>27</v>
       </c>
@@ -4017,8 +4482,11 @@
       <c r="G160" s="5">
         <v>398.31847119399998</v>
       </c>
-    </row>
-    <row r="161" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H160" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="161" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A161" s="2">
         <v>28</v>
       </c>
@@ -4040,8 +4508,11 @@
       <c r="G161" s="5">
         <v>412.33412122800001</v>
       </c>
-    </row>
-    <row r="162" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H161" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="162" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A162" s="2">
         <v>29</v>
       </c>
@@ -4063,8 +4534,11 @@
       <c r="G162" s="5">
         <v>426.34977126199999</v>
       </c>
-    </row>
-    <row r="163" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H162" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="163" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A163" s="2">
         <v>30</v>
       </c>
@@ -4085,6 +4559,9 @@
       </c>
       <c r="G163" s="5">
         <v>440.36542129599997</v>
+      </c>
+      <c r="H163" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>